<commit_message>
Correction de l'input user dans ouidef.jsp
</commit_message>
<xml_diff>
--- a/compte des heures.xlsx
+++ b/compte des heures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viann\Documents\CentraleNantes\Cours2eAnnée\PGROU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1951BAC4-EBD6-4A17-92F3-3764BD015D42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565D21AF-603D-4F09-87AE-1948D6AE4E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{12C2BD03-25CC-413B-88DD-64BD17DE13FD}"/>
   </bookViews>
@@ -107,13 +107,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,20 +456,20 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
   <sheetData>
     <row r="1" spans="1:6" ht="28.75" customHeight="1" x14ac:dyDescent="0.75">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.75">
       <c r="B3" t="s">
@@ -495,32 +495,42 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="B7">
+        <v>8</v>
+      </c>
+    </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.75">
-      <c r="G19" s="2">
+      <c r="G19" s="3">
         <f>SUM(B20:E20)</f>
-        <v>14</v>
-      </c>
-      <c r="H19" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.75">
-      <c r="B20" s="3">
+      <c r="B20" s="1">
         <f>SUM(B4:B19)</f>
-        <v>14</v>
-      </c>
-      <c r="C20" s="3">
+        <v>26</v>
+      </c>
+      <c r="C20" s="1">
         <f t="shared" ref="C20:E20" si="0">SUM(C4:C19)</f>
         <v>0</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Page de choix des dates de la mission logement faite
</commit_message>
<xml_diff>
--- a/compte des heures.xlsx
+++ b/compte des heures.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viann\Documents\CentraleNantes\Cours2eAnnée\PGROU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{565D21AF-603D-4F09-87AE-1948D6AE4E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E933641E-3EEC-4C03-9ED3-5E60544833B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10980" xr2:uid="{12C2BD03-25CC-413B-88DD-64BD17DE13FD}"/>
+    <workbookView xWindow="4800" yWindow="335" windowWidth="14400" windowHeight="7830" xr2:uid="{12C2BD03-25CC-413B-88DD-64BD17DE13FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
     <t>Zoé</t>
   </si>
   <si>
-    <t>On inscrit le nombre d'heures régulièrement… Le contenu du travail n'est pas important !</t>
+    <t>On inscrit le nombre d'heures régulièrement… Le contenu du travail n'est pas important</t>
   </si>
 </sst>
 </file>
@@ -456,7 +456,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -505,17 +505,22 @@
         <v>8</v>
       </c>
     </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="B8">
+        <v>4</v>
+      </c>
+    </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.75">
       <c r="G19" s="3">
         <f>SUM(B20:E20)</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.75">
       <c r="B20" s="1">
         <f>SUM(B4:B19)</f>
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ref="C20:E20" si="0">SUM(C4:C19)</f>

</xml_diff>

<commit_message>
Suppression de la bdd par la VE possible et création de la page gestion admin
</commit_message>
<xml_diff>
--- a/compte des heures.xlsx
+++ b/compte des heures.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viann\Documents\CentraleNantes\Cours2eAnnée\PGROU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E933641E-3EEC-4C03-9ED3-5E60544833B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF6FB681-DA2F-4BF5-A6EB-AF6E4E760701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4800" yWindow="335" windowWidth="14400" windowHeight="7830" xr2:uid="{12C2BD03-25CC-413B-88DD-64BD17DE13FD}"/>
   </bookViews>
@@ -455,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DDCD9A-1BFE-4C27-9ECC-4EE953CF5C56}">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -510,17 +510,22 @@
         <v>4</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.75">
+      <c r="B9">
+        <v>6</v>
+      </c>
+    </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.75">
       <c r="G19" s="3">
         <f>SUM(B20:E20)</f>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.75">
       <c r="B20" s="1">
         <f>SUM(B4:B19)</f>
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ref="C20:E20" si="0">SUM(C4:C19)</f>

</xml_diff>

<commit_message>
Evolution chemin relatif import commune
</commit_message>
<xml_diff>
--- a/compte des heures.xlsx
+++ b/compte des heures.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viann\Documents\CentraleNantes\Cours2eAnnée\pappl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\viann\Documents\CentraleNantes\Cours2eAnnée\PGROU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42D4E1DF-B866-43E9-8E8F-402F9B685831}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B727204-2879-46F1-8F0D-C141982FC1F7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{12C2BD03-25CC-413B-88DD-64BD17DE13FD}"/>
   </bookViews>
@@ -451,7 +451,7 @@
   <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
@@ -515,17 +515,22 @@
         <v>8</v>
       </c>
     </row>
+    <row r="11" spans="1:6">
+      <c r="B11">
+        <v>5</v>
+      </c>
+    </row>
     <row r="19" spans="2:8">
       <c r="G19" s="3">
         <f>SUM(B20:E20)</f>
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="H19" s="3"/>
     </row>
     <row r="20" spans="2:8">
       <c r="B20" s="1">
         <f>SUM(B4:B19)</f>
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" ref="C20:E20" si="0">SUM(C4:C19)</f>

</xml_diff>